<commit_message>
Removing all the data points with less than 24 hours of on stream hours to get better datapoints
</commit_message>
<xml_diff>
--- a/Model Scores.xlsx
+++ b/Model Scores.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spect\OneDrive\Desktop\ML_conda_projects\spectre_lab\volve_dataset_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88095675-2B0F-4EE4-A7B5-DE869A2CC682}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78535A2A-671C-4BAC-B6F8-242AAB19F816}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="v5" sheetId="1" r:id="rId1"/>
+    <sheet name="v6" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="32">
   <si>
     <t>Train</t>
   </si>
@@ -102,15 +103,6 @@
     <t>LSTM RNN</t>
   </si>
   <si>
-    <t>[30 (bi),10 (bi),1], w = 2, b = 32, epochs = 550</t>
-  </si>
-  <si>
-    <t>[30 (bi),10 (bi),1], w = 3, b = 10, epochs = 250</t>
-  </si>
-  <si>
-    <t>[30 (bi),10 (bi),1], w = 3, b = 10, epochs = 140</t>
-  </si>
-  <si>
     <t>GRU RNN</t>
   </si>
   <si>
@@ -118,6 +110,18 @@
   </si>
   <si>
     <t>Test</t>
+  </si>
+  <si>
+    <t>[30 (bi),10 (bi),1], w = 2, b = 20</t>
+  </si>
+  <si>
+    <t>[30 (bi),10 (bi),1], w = 3, b = 32</t>
+  </si>
+  <si>
+    <t>[30 (bi),10 (bi),1], w = 5, b = 16</t>
+  </si>
+  <si>
+    <t>[30 (bi),10 (bi),1], w = 3, b = 16</t>
   </si>
 </sst>
 </file>
@@ -206,7 +210,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -238,6 +242,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -518,10 +526,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -552,7 +560,7 @@
         <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E2" s="12"/>
     </row>
@@ -583,7 +591,7 @@
         <v>7.35</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -707,13 +715,13 @@
         <v>21</v>
       </c>
       <c r="B13" s="5">
-        <v>3.21</v>
+        <v>6.46</v>
       </c>
       <c r="C13" s="5">
-        <v>1.41</v>
+        <v>1.08</v>
       </c>
       <c r="D13" s="3">
-        <v>12.38</v>
+        <v>10.59</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>22</v>
@@ -724,16 +732,16 @@
         <v>23</v>
       </c>
       <c r="B14" s="5">
-        <v>1.35</v>
+        <v>300.64999999999998</v>
       </c>
       <c r="C14" s="5">
-        <v>2.8</v>
+        <v>1.31</v>
       </c>
       <c r="D14" s="3">
-        <v>142.24</v>
+        <v>48.45</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -741,33 +749,67 @@
         <v>24</v>
       </c>
       <c r="B15" s="5">
-        <v>1.31</v>
+        <v>21.97</v>
       </c>
       <c r="C15" s="5">
-        <v>1.2</v>
+        <v>0.83</v>
       </c>
       <c r="D15" s="3">
-        <v>17.920000000000002</v>
+        <v>5.64</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="5">
+        <v>5.71</v>
+      </c>
+      <c r="C16" s="5">
+        <v>0.71</v>
+      </c>
+      <c r="D16" s="3">
+        <v>7.9</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="5">
+        <v>12.9</v>
+      </c>
+      <c r="C17" s="5">
+        <v>0.72</v>
+      </c>
+      <c r="D17" s="3">
+        <v>17.66</v>
+      </c>
+      <c r="E17" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="5">
-        <v>1.51</v>
-      </c>
-      <c r="C16" s="5">
-        <v>1.5</v>
-      </c>
-      <c r="D16" s="3">
-        <v>38.21</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>27</v>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="5">
+        <v>4.92</v>
+      </c>
+      <c r="C18" s="5">
+        <v>0.82</v>
+      </c>
+      <c r="D18" s="3">
+        <v>21.24</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -779,4 +821,229 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31F8548A-02B6-4FF9-BF50-0BEE2358AA93}">
+  <dimension ref="A1:E18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.88671875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="46.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="10"/>
+      <c r="B2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="12"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="14">
+        <v>4.54</v>
+      </c>
+      <c r="C3" s="14">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D3" s="14"/>
+      <c r="E3" s="3"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="14"/>
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="14"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="3"/>
+    </row>
+    <row r="11" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="3"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="14"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="14"/>
+      <c r="C15" s="14"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="14"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="14"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
+      <c r="E17" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:E2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Re-starting the process of feature engineering
</commit_message>
<xml_diff>
--- a/Model Scores.xlsx
+++ b/Model Scores.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spect\OneDrive\Desktop\ML_conda_projects\spectre_lab\volve_dataset_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78535A2A-671C-4BAC-B6F8-242AAB19F816}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96AB590E-C153-4448-8462-FCAD081D90CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12192" yWindow="2556" windowWidth="17280" windowHeight="8880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="v5" sheetId="1" r:id="rId1"/>
     <sheet name="v6" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="33">
   <si>
     <t>Train</t>
   </si>
@@ -122,13 +123,16 @@
   </si>
   <si>
     <t>[30 (bi),10 (bi),1], w = 3, b = 16</t>
+  </si>
+  <si>
+    <t>R2_score</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -136,8 +140,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -153,6 +165,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -210,7 +234,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -227,6 +251,19 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -242,10 +279,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -539,20 +590,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="11" t="s">
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="20" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="10"/>
+      <c r="A2" s="19"/>
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
@@ -562,7 +613,7 @@
       <c r="D2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="12"/>
+      <c r="E2" s="21"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
@@ -825,223 +876,315 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31F8548A-02B6-4FF9-BF50-0BEE2358AA93}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.88671875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="46.5546875" customWidth="1"/>
+    <col min="1" max="1" width="15.88671875" style="16" customWidth="1"/>
+    <col min="2" max="4" width="8.88671875" style="9"/>
+    <col min="5" max="7" width="8.88671875" style="11"/>
+    <col min="8" max="8" width="46.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="11" t="s">
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="25" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="10"/>
-      <c r="B2" s="3" t="s">
+    <row r="2" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="23"/>
+      <c r="B2" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="E2" s="12"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="13" t="s">
+      <c r="E2" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="H2" s="26"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="14">
+      <c r="B3" s="8">
         <v>4.54</v>
       </c>
-      <c r="C3" s="14">
+      <c r="C3" s="8">
         <v>2.2000000000000002</v>
       </c>
-      <c r="D3" s="14"/>
-      <c r="E3" s="3"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="13" t="s">
+      <c r="D3" s="8"/>
+      <c r="E3" s="10">
+        <v>0.95</v>
+      </c>
+      <c r="F3" s="10">
+        <v>0.34</v>
+      </c>
+      <c r="G3" s="10"/>
+      <c r="H3" s="3"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="3" t="s">
+      <c r="B4" s="8">
+        <v>3.45</v>
+      </c>
+      <c r="C4" s="8">
+        <v>0.99</v>
+      </c>
+      <c r="D4" s="8"/>
+      <c r="E4" s="10">
+        <v>0.96</v>
+      </c>
+      <c r="F4" s="10">
+        <v>0.7</v>
+      </c>
+      <c r="G4" s="10"/>
+      <c r="H4" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="13" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="14"/>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="3" t="s">
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="13" t="s">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="3" t="s">
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="13" t="s">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="3" t="s">
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
+      <c r="H7" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="13" t="s">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="3" t="s">
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="13" t="s">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="14"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="14"/>
-      <c r="E9" s="3" t="s">
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="13" t="s">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="3"/>
-    </row>
-    <row r="11" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="13" t="s">
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="3"/>
+    </row>
+    <row r="11" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="3"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="13" t="s">
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="3"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="3" t="s">
+      <c r="B12" s="8">
+        <v>14.93</v>
+      </c>
+      <c r="C12" s="8">
+        <v>6.13</v>
+      </c>
+      <c r="D12" s="8"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="13" t="s">
+    <row r="13" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="14"/>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="3" t="s">
+      <c r="B13" s="8">
+        <v>1.87</v>
+      </c>
+      <c r="C13" s="8">
+        <v>1.19</v>
+      </c>
+      <c r="D13" s="8"/>
+      <c r="E13" s="10">
+        <v>0.98</v>
+      </c>
+      <c r="F13" s="10">
+        <v>0.64</v>
+      </c>
+      <c r="G13" s="10"/>
+      <c r="H13" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="13" t="s">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="14"/>
-      <c r="C14" s="14"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="3" t="s">
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="13" t="s">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="14"/>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="3" t="s">
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="10"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="13" t="s">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="3" t="s">
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="13" t="s">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="3" t="s">
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="13" t="s">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="3" t="s">
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10"/>
+      <c r="G18" s="10"/>
+      <c r="H18" s="3" t="s">
         <v>31</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:D1"/>
-    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="E1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>